<commit_message>
UI get symptoms finished
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Weights.xlsx
+++ b/src/main/resources/files/Weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalia/Documents/CEU/Asignaturas/SistemasSoporte/AnemiaDSS/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F1C7D9-8357-C049-B34F-556D88B498A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DE633-602F-7C42-A78A-9F7AB4B4D84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>Craneal balloning</t>
   </si>
   <si>
-    <t xml:space="preserve">Aplastic crisis </t>
-  </si>
-  <si>
     <t>Bacterial infectons</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>Chronic_disease_anemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplasic crisis </t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1168,51 +1168,51 @@
         <v>43</v>
       </c>
       <c r="AS1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AU1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AV1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AW1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AX1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AY1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BB1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="BC1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="6" t="s">
+      <c r="BD1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="6" t="s">
+      <c r="BE1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="BE1" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="14">
         <v>10838</v>
@@ -1284,22 +1284,22 @@
         <v>0</v>
       </c>
       <c r="Z2" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA2" s="14">
         <v>11663</v>
       </c>
       <c r="AB2" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC2" s="11">
         <v>4163</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="14">
         <v>6663</v>
@@ -1311,7 +1311,7 @@
         <v>8338</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ2" s="14">
         <v>9162</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="3" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="24">
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="25">
         <v>0</v>
@@ -1433,31 +1433,31 @@
         <v>0</v>
       </c>
       <c r="R3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="25">
+        <v>0</v>
+      </c>
+      <c r="T3" s="27">
+        <v>0</v>
+      </c>
+      <c r="U3" s="28">
+        <v>0</v>
+      </c>
+      <c r="V3" s="27">
+        <v>0</v>
+      </c>
+      <c r="W3" s="28">
+        <v>0</v>
+      </c>
+      <c r="X3" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="28">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="S3" s="25">
-        <v>0</v>
-      </c>
-      <c r="T3" s="27">
-        <v>0</v>
-      </c>
-      <c r="U3" s="28">
-        <v>0</v>
-      </c>
-      <c r="V3" s="27">
-        <v>0</v>
-      </c>
-      <c r="W3" s="28">
-        <v>0</v>
-      </c>
-      <c r="X3" s="27">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="28">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="AA3" s="15">
         <v>3813</v>
@@ -1490,7 +1490,7 @@
         <v>1907</v>
       </c>
       <c r="AK3" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AL3" s="30">
         <v>0</v>
@@ -1499,7 +1499,7 @@
         <v>11427</v>
       </c>
       <c r="AN3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO3" s="29">
         <v>0</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="4" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="16">
         <v>7143</v>
@@ -1588,7 +1588,7 @@
         <v>4286</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M4" s="16">
         <v>3333</v>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="16">
         <v>5714</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="Z4" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA4" s="36">
         <v>0</v>
@@ -1687,7 +1687,7 @@
         <v>1429</v>
       </c>
       <c r="AS4" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AT4" s="37">
         <v>0</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="5" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="38">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>12086</v>
       </c>
       <c r="T5" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U5" s="39">
         <v>0</v>
@@ -1854,22 +1854,22 @@
         <v>10986</v>
       </c>
       <c r="AQ5" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AR5" s="17">
         <v>14286</v>
       </c>
       <c r="AS5" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT5" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="AT5" s="44" t="s">
+      <c r="AU5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AU5" s="12" t="s">
+      <c r="AV5" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="AV5" s="12" t="s">
-        <v>77</v>
       </c>
       <c r="AW5" s="17">
         <v>13186</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="6" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="45">
         <v>0</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="7" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="14">
         <v>9886</v>
@@ -2107,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M7" s="14">
         <v>13186</v>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S7" s="20">
         <v>0</v>
@@ -2173,64 +2173,64 @@
         <v>0</v>
       </c>
       <c r="AH7" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="AI7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="11" t="s">
+      <c r="AK7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="AK7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AY7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="11" t="s">
+      <c r="BA7" s="19" t="s">
         <v>76</v>
-      </c>
-      <c r="BA7" s="19" t="s">
-        <v>77</v>
       </c>
       <c r="BB7" s="19">
         <v>0</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="8" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="24">
         <v>0</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="9" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="33">
         <v>0</v>
@@ -2432,112 +2432,112 @@
         <v>0</v>
       </c>
       <c r="E9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="31">
+        <v>0</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="33">
+        <v>0</v>
+      </c>
+      <c r="M9" s="33">
+        <v>0</v>
+      </c>
+      <c r="N9" s="33">
+        <v>0</v>
+      </c>
+      <c r="O9" s="33">
+        <v>0</v>
+      </c>
+      <c r="P9" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="33">
+        <v>0</v>
+      </c>
+      <c r="R9" s="31">
+        <v>0</v>
+      </c>
+      <c r="S9" s="31">
+        <v>0</v>
+      </c>
+      <c r="T9" s="34">
+        <v>0</v>
+      </c>
+      <c r="U9" s="35">
+        <v>0</v>
+      </c>
+      <c r="V9" s="34">
+        <v>0</v>
+      </c>
+      <c r="W9" s="35">
+        <v>0</v>
+      </c>
+      <c r="X9" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="31">
-        <v>0</v>
-      </c>
-      <c r="G9" s="31">
-        <v>0</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="AA9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="33">
-        <v>0</v>
-      </c>
-      <c r="J9" s="31">
-        <v>0</v>
-      </c>
-      <c r="K9" s="16" t="s">
+      <c r="AI9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="33">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN9" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="L9" s="33">
-        <v>0</v>
-      </c>
-      <c r="M9" s="33">
-        <v>0</v>
-      </c>
-      <c r="N9" s="33">
-        <v>0</v>
-      </c>
-      <c r="O9" s="33">
-        <v>0</v>
-      </c>
-      <c r="P9" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="33">
-        <v>0</v>
-      </c>
-      <c r="R9" s="31">
-        <v>0</v>
-      </c>
-      <c r="S9" s="31">
-        <v>0</v>
-      </c>
-      <c r="T9" s="34">
-        <v>0</v>
-      </c>
-      <c r="U9" s="35">
-        <v>0</v>
-      </c>
-      <c r="V9" s="34">
-        <v>0</v>
-      </c>
-      <c r="W9" s="35">
-        <v>0</v>
-      </c>
-      <c r="X9" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA9" s="33">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="33">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="33">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH9" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="33">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN9" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="AO9" s="31">
         <v>0</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="10" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="38">
         <v>0</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="11" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="18">
         <v>13186</v>
@@ -2862,76 +2862,76 @@
         <v>7686</v>
       </c>
       <c r="AG11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AH11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AN11" s="13" t="s">
+      <c r="AO11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="46">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="45">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="AO11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AW11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="46">
-        <v>0</v>
-      </c>
-      <c r="AY11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AZ11" s="50" t="s">
+      <c r="BA11" s="45">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="BA11" s="45">
-        <v>0</v>
-      </c>
-      <c r="BB11" s="13" t="s">
+      <c r="BC11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="BC11" s="45" t="s">
+      <c r="BD11" s="45" t="s">
         <v>76</v>
-      </c>
-      <c r="BD11" s="45" t="s">
-        <v>77</v>
       </c>
       <c r="BE11" s="46">
         <v>0</v>

</xml_diff>

<commit_message>
i tried menu, solved weightsxlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Weights.xlsx
+++ b/src/main/resources/files/Weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalia/Documents/CEU/Asignaturas/SistemasSoporte/AnemiaDSS/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45663992-F4AA-5248-A307-ACE90B6EE27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA090A5-A708-6744-9E87-909332D160D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>ANEMIA/SYMPTOMS</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Polycythemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Anemic_syndrome_FEMALE</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1016,7 @@
   <dimension ref="A1:BE22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1370,7 +1373,7 @@
     </row>
     <row r="3" spans="1:57" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B3" s="10">
         <v>12.5</v>

</xml_diff>